<commit_message>
ajout du package test pour JUNIT
</commit_message>
<xml_diff>
--- a/Journal de travail - Aurélien May.xlsx
+++ b/Journal de travail - Aurélien May.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurel\OneDrive\Desktop\Aurélien\OneDrive\HEVS\S2\POO\ProjetSmartphone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="11_B5CCD2F72FE37CE26E339E56ADDC14C75C28AAEB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9ADC5AE7-9C0F-4891-93A4-E1452255AC2D}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_B5CCD2F72FE37CE26E339E56ADDC14C75C28AAEB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{44309BB1-D4B7-4B1B-BD19-9F13D12977AF}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Journal de tavail individuel </t>
   </si>
@@ -54,27 +54,13 @@
     <t>Frame</t>
   </si>
   <si>
-    <t>Menu (home)</t>
-  </si>
-  <si>
     <t>Détails des tâches</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Heure de travail (en h)</t>
-  </si>
-  <si>
     <t>Applications</t>
-  </si>
-  <si>
-    <t>Vous trouverez ci-dessous mon temps de travail pour chacune des "applications".</t>
-  </si>
-  <si>
-    <t>- Interface graphique
-- Algorythme
-- Exceptions (division par 0)</t>
   </si>
   <si>
     <t>- Interface graphique</t>
@@ -89,14 +75,42 @@
 - Suppression d'images</t>
   </si>
   <si>
-    <t>Barre de contrôle (nom réseau, heure, signal)</t>
-  </si>
-  <si>
     <t>Javadoc + diverses modifications</t>
   </si>
   <si>
     <t>- Ajout des commentaires
 - Optimisation du code</t>
+  </si>
+  <si>
+    <t>- Interface graphique
+- Algorythme</t>
+  </si>
+  <si>
+    <t>Vous trouverez ci-dessous mon temps de travail pour chacune des classes.</t>
+  </si>
+  <si>
+    <t>PanelEcranCenter
+PanelEcranNorth</t>
+  </si>
+  <si>
+    <t>IconButton
+IconPanel</t>
+  </si>
+  <si>
+    <t>- Exceptions
+- Image draw
+- Méthodes</t>
+  </si>
+  <si>
+    <t>- Interface graphique (applications, disposition,…)
+- SSID, signal
+- Heure</t>
+  </si>
+  <si>
+    <t>Heure de travail</t>
+  </si>
+  <si>
+    <t>JUNIT</t>
   </si>
 </sst>
 </file>
@@ -140,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -316,44 +330,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,9 +345,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -409,13 +387,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -732,109 +704,116 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" s="11" customFormat="1" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>8</v>
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>25</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>13</v>
+      <c r="C9" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
+      <c r="A10" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="4">
+        <v>25</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4">
-        <v>8</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="A12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="4">
+        <v>8</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4">
         <v>5</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="7">
-        <v>25</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="C14" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="4">
         <v>4</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="11" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="8">
-        <f>SUM(B9:B15)</f>
-        <v>97</v>
-      </c>
-      <c r="C16" s="10"/>
+    <row r="16" spans="1:3" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="10" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7">
+        <f>SUM(B9:B16)</f>
+        <v>96</v>
+      </c>
+      <c r="C17" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>